<commit_message>
All reports added and updated
</commit_message>
<xml_diff>
--- a/testdata/Scenario1_Output.xlsx
+++ b/testdata/Scenario1_Output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="9">
   <si>
     <t>Company Name</t>
   </si>
@@ -91,7 +91,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
         <v>4</v>

</xml_diff>